<commit_message>
Minor revision to the sleep example.
</commit_message>
<xml_diff>
--- a/docs/Data/sleep.xlsx
+++ b/docs/Data/sleep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\docs\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\BYUI_M221_Book_R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD96A7E-2193-41CD-A95E-BC09E7077ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD95638-61C8-4721-9487-16EDB70ABAFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8205" windowWidth="29040" windowHeight="16440" xr2:uid="{5AAE2C05-1A98-47C3-B116-2BD3185D8199}"/>
   </bookViews>

</xml_diff>